<commit_message>
Params - comments update
</commit_message>
<xml_diff>
--- a/doc/Params.xlsx
+++ b/doc/Params.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="717">
   <si>
     <t>OP6_Scaling_mode</t>
   </si>
@@ -2207,6 +2207,12 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>1=negative detune</t>
+  </si>
+  <si>
+    <t>It maps to ReverbSend for the current MiniDexed version (today: 2023.01.15)</t>
   </si>
 </sst>
 </file>
@@ -2248,7 +2254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2257,6 +2263,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2577,7 +2586,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,7 +2597,7 @@
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2671,7 +2680,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2771,7 +2783,7 @@
         <v>127</v>
       </c>
       <c r="F9" s="4">
-        <v>12</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2914,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2974,7 +2986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -3054,7 +3066,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -3074,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -3094,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -3111,10 +3123,10 @@
         <v>127</v>
       </c>
       <c r="F26" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -3133,8 +3145,11 @@
       <c r="F27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="5" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -3154,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -3174,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -3194,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -3214,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>

</xml_diff>